<commit_message>
DETC-104 - Updating section 3 - design 2  implementation details
</commit_message>
<xml_diff>
--- a/section_2_databases/DataModel.xlsx
+++ b/section_2_databases/DataModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santhoshjanakiraman/Personal/Projects/gvtech/sg-gvt-detc/sg-gvt-detc/section_2_databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76674B85-F2A9-0E43-85E2-58538C130CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC1B2BF-4614-734B-8357-75D7609269F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3100" windowWidth="37260" windowHeight="21100" activeTab="1" xr2:uid="{1E3F73C2-CE41-0D41-8375-B81EAD1E82BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="79">
   <si>
     <t>tItemDetails</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>UserId</t>
-  </si>
-  <si>
-    <t>ContactTypeId</t>
   </si>
 </sst>
 </file>
@@ -646,7 +643,7 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F25" sqref="F24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,7 +953,7 @@
   <dimension ref="A2:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,15 +1039,15 @@
       <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>79</v>
+      <c r="L3" t="s">
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N49" si="2">CONCATENATE(K3,L3,M3)</f>
-        <v>(ContactTypeId int</v>
+        <f>CONCATENATE(K4,L3,M3)</f>
+        <v>,ContactTypeCode varchar(20)</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1084,14 +1081,14 @@
         <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="2"/>
-        <v>,ContactTypeCode varchar(20)</v>
+        <f>CONCATENATE(K5,L4,M4)</f>
+        <v>,ContactTypeDesc varchar(100)</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1125,14 +1122,14 @@
         <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N5" t="str">
-        <f>CONCATENATE(K5,L5,M5)</f>
-        <v>,ContactTypeDesc varchar(100)</v>
+        <f>CONCATENATE(K6,L5,M5)</f>
+        <v>,IsActive varchar(1)</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1166,14 +1163,14 @@
         <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N6" t="str">
-        <f>CONCATENATE(K6,L6,M6)</f>
-        <v>,IsActive varchar(1)</v>
+        <f>CONCATENATE(K7,L6,M6)</f>
+        <v>,CreatedBy varchar(20)</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1207,14 +1204,14 @@
         <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="N7" t="str">
-        <f>CONCATENATE(K7,L7,M7)</f>
-        <v>,CreatedBy varchar(20)</v>
+        <f>CONCATENATE(K8,L7,M7)</f>
+        <v>,CreatedDate timestamp</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1248,14 +1245,14 @@
         <v>57</v>
       </c>
       <c r="L8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="N8" t="str">
-        <f>CONCATENATE(K8,L8,M8)</f>
-        <v>,CreatedDate timestamp</v>
+        <f>CONCATENATE(K9,L8,M8)</f>
+        <v>,UpdatedBy varchar(20)</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1283,14 +1280,14 @@
         <v>57</v>
       </c>
       <c r="L9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="N9" t="str">
-        <f>CONCATENATE(K9,L9,M9)</f>
-        <v>,UpdatedBy varchar(20)</v>
+        <f>CONCATENATE(K10,L9,M9)</f>
+        <v>UpdatedDate timestamp</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1317,18 +1314,12 @@
         <f>CONCATENATE(F10,G10,H10)</f>
         <v>CREATE TABLE tMasterContactDetails</v>
       </c>
-      <c r="K10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" t="s">
-        <v>16</v>
-      </c>
       <c r="M10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N10" t="str">
-        <f>CONCATENATE(K10,L10,M10)</f>
-        <v>,UpdatedDate timestamp</v>
+        <f>CONCATENATE(K11,L10,M10)</f>
+        <v>);</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1358,13 +1349,6 @@
         <f>CONCATENATE(F11,G11,H11)</f>
         <v>(ContactId int</v>
       </c>
-      <c r="M11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N11" t="str">
-        <f>CONCATENATE(K11,L11,M11)</f>
-        <v>);</v>
-      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1422,7 +1406,7 @@
         <v>37</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="N3:N49" si="2">CONCATENATE(K13,L13,M13)</f>
         <v>CREATE TABLE tRefWeightScale</v>
       </c>
     </row>

</xml_diff>